<commit_message>
Nave principal vai ser essa!
</commit_message>
<xml_diff>
--- a/tudin.xlsx
+++ b/tudin.xlsx
@@ -25,10 +25,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -104,6 +110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DX64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AE24" sqref="AE24"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AF29" sqref="AF29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9883,23 +9890,23 @@
         <f t="shared" si="32"/>
         <v>7536</v>
       </c>
-      <c r="AD30" s="4">
+      <c r="AD30" s="8">
         <f t="shared" si="33"/>
         <v>7540</v>
       </c>
-      <c r="AE30" s="4">
+      <c r="AE30" s="8">
         <f t="shared" si="34"/>
         <v>7544</v>
       </c>
-      <c r="AF30" s="4">
+      <c r="AF30" s="8">
         <f t="shared" si="35"/>
         <v>7548</v>
       </c>
-      <c r="AG30" s="4">
+      <c r="AG30" s="8">
         <f t="shared" si="36"/>
         <v>7552</v>
       </c>
-      <c r="AH30" s="4">
+      <c r="AH30" s="8">
         <f t="shared" si="37"/>
         <v>7556</v>
       </c>

</xml_diff>